<commit_message>
corrected minor bugs in plots and data
</commit_message>
<xml_diff>
--- a/in/verifications/series_S.xlsx
+++ b/in/verifications/series_S.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\eclipse\workspaces\Extraction\Datapol\in\verifications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Extraction\Datapol\in\verifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F92A0DE-B551-4FBA-A3ED-D8A8DFA52BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E4FB6613-F1B5-4170-A0FF-89DED8DEA140}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$128</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="141">
   <si>
     <t>Code departement</t>
   </si>
@@ -394,12 +393,75 @@
   </si>
   <si>
     <t>probablement à vérifier manuellement</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>9D</t>
+  </si>
+  <si>
+    <t>9E</t>
+  </si>
+  <si>
+    <t>9F</t>
+  </si>
+  <si>
+    <t>9G</t>
+  </si>
+  <si>
+    <t>9H</t>
+  </si>
+  <si>
+    <t>9J</t>
+  </si>
+  <si>
+    <t>9K</t>
+  </si>
+  <si>
+    <t>9L</t>
+  </si>
+  <si>
+    <t>9M</t>
+  </si>
+  <si>
+    <t>9N</t>
+  </si>
+  <si>
+    <t>9P</t>
+  </si>
+  <si>
+    <t>9R</t>
+  </si>
+  <si>
+    <t>ZZC</t>
+  </si>
+  <si>
+    <t>ZZS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +525,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,22 +841,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D88A98-4F04-4867-8AAF-B535A0430EF2}">
-  <dimension ref="A1:D109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -813,7 +878,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -824,7 +889,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -835,7 +900,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -846,7 +911,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -857,7 +922,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -868,7 +933,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -879,7 +944,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -890,7 +955,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -901,7 +966,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -912,7 +977,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -923,7 +988,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -934,7 +999,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -945,7 +1010,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -956,7 +1021,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
@@ -967,7 +1032,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -978,7 +1043,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
@@ -989,7 +1054,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1000,7 +1065,7 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1011,551 +1076,551 @@
         <v>2008.2013999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1958.1962000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C24" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C54" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="B56" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C56" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+      <c r="B58" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C58" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+      <c r="B63" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C64" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
+      <c r="B65" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C65" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+      <c r="B66" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+      <c r="B67" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C67" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+      <c r="B68" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
+      <c r="B69" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" s="4">
-        <v>2004.2013999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>114</v>
@@ -1564,9 +1629,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>114</v>
@@ -1575,9 +1640,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>114</v>
@@ -1586,9 +1651,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>114</v>
@@ -1597,9 +1662,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>114</v>
@@ -1608,9 +1673,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>114</v>
@@ -1618,13 +1683,10 @@
       <c r="C75" s="4">
         <v>2004.2013999999999</v>
       </c>
-      <c r="D75" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>114</v>
@@ -1632,43 +1694,46 @@
       <c r="C76" s="4">
         <v>2004.2013999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D76" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77" s="4">
+        <v>2004.2013999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C79" s="4">
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>113</v>
@@ -1677,20 +1742,20 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C81" s="4">
-        <v>2004.2013999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>114</v>
@@ -1699,9 +1764,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>114</v>
@@ -1710,31 +1775,31 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C84" s="4">
-        <v>2004.2013999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1958.1962000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C85" s="4">
-        <v>2004.2013999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1958.1962000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>114</v>
@@ -1743,9 +1808,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>114</v>
@@ -1754,9 +1819,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>114</v>
@@ -1765,9 +1830,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>114</v>
@@ -1776,9 +1841,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>114</v>
@@ -1787,9 +1852,9 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>114</v>
@@ -1798,202 +1863,433 @@
         <v>2004.2013999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C92" s="4">
+        <v>2004.2013999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C93" s="4">
+        <v>2004.2013999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C94" s="4">
+        <v>2004.2013999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C92" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
+      <c r="B95" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C102" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C103" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C106" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C108" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" s="4">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C113" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="2" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C115" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C116" s="4">
+        <v>1958.1962000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="2" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C100" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
+      <c r="B119" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C101" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="2" t="s">
+      <c r="B120" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C121" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" s="2" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C103" s="4">
-        <v>2011.2017000000001</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" s="2" t="s">
+      <c r="B122" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122" s="4">
+        <v>2011.2017000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C104" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" s="2" t="s">
+      <c r="B123" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" s="2" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C106" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
+      <c r="B125" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C125" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C107" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" s="2" t="s">
+      <c r="B126" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C126" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C108" s="4">
-        <v>2008.2013999999999</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
+      <c r="B127" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C127" s="4">
+        <v>2008.2013999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C128" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D128" s="6" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" s="4">
+        <v>1959.1967999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C130" s="4">
+        <v>1965.1974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>